<commit_message>
updated some data labels & files
</commit_message>
<xml_diff>
--- a/LANDIS_stuff/refined_species_list_for_LANDIS_initialcommunities_4Jan2022_COLORCODED.xlsx
+++ b/LANDIS_stuff/refined_species_list_for_LANDIS_initialcommunities_4Jan2022_COLORCODED.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theha\Documents\mastersthesis_repo\mastersthesis\LANDIS_stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{473A5A01-702C-4C49-A758-C7D39731381E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8EAF34-26CC-48EE-BDF8-A71070706790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="refined_species_list_for_LANDIS" sheetId="1" r:id="rId1"/>
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1126,11 +1126,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1474,17 +1474,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
+    <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
         <v>761</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="1" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>